<commit_message>
att cadastro, Certificado_selo, contato, FAQ, inserção_dados, login, meuperfil, pag_inicial, pontos_coleta and relatorios
atualizações
</commit_message>
<xml_diff>
--- a/Usuarios_Cadastrados.xlsx
+++ b/Usuarios_Cadastrados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,38 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EmpresaTeste</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>12.345.678/9123-45</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12345-678</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>eg@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>(71) 99945-2004</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Eg2024!</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>